<commit_message>
revisiting a year later
</commit_message>
<xml_diff>
--- a/Data/Benthic sediment characterization -compare to D Whitall.xlsx
+++ b/Data/Benthic sediment characterization -compare to D Whitall.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Fagaalu-Sedimentation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.messina\Documents\GitHub\Fagaalu-Sedimentation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66835BB1-B117-4A6D-817D-83A1DCDBDD17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="690" windowWidth="24435" windowHeight="11250" activeTab="2"/>
+    <workbookView xWindow="11028" yWindow="3972" windowWidth="17280" windowHeight="9108" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,12 +18,23 @@
     <sheet name="Benthic_sediment_characterizati" sheetId="3" r:id="rId3"/>
     <sheet name="LOI" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="95">
   <si>
     <t>Sites</t>
   </si>
@@ -295,12 +307,24 @@
   </si>
   <si>
     <t>3A</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Org</t>
+  </si>
+  <si>
+    <t>Carb</t>
+  </si>
+  <si>
+    <t>Terrig</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000000000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -343,7 +367,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -360,25 +384,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -387,6 +472,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,6 +592,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -515,6 +644,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -690,23 +836,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F65536"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -726,7 +872,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -740,7 +886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -754,7 +900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -768,7 +914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -788,7 +934,7 @@
         <v>-14.2907720315</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -808,7 +954,7 @@
         <v>-14.2913519202</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -828,7 +974,7 @@
         <v>-14.291131522500001</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -848,7 +994,7 @@
         <v>-14.2897126905</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -868,7 +1014,7 @@
         <v>-14.2909125717</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -888,7 +1034,7 @@
         <v>-14.2897257644</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -908,7 +1054,7 @@
         <v>-14.2926303124</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -928,7 +1074,7 @@
         <v>-14.2925835986</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -948,7 +1094,7 @@
         <v>-14.2920813863</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -968,7 +1114,7 @@
         <v>-14.289224685100001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -988,7 +1134,7 @@
         <v>-14.2904269686</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1008,7 +1154,7 @@
         <v>-14.289821587900001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1028,7 +1174,7 @@
         <v>-14.291256342300001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1048,7 +1194,7 @@
         <v>-14.291420175500001</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1068,7 +1214,7 @@
         <v>-14.290662125300001</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1088,7 +1234,7 @@
         <v>-14.2915457557</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1108,7 +1254,7 @@
         <v>-14.2903972341</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1128,7 +1274,7 @@
         <v>-14.288742795199999</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1148,7 +1294,7 @@
         <v>-14.293183777499999</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1168,7 +1314,7 @@
         <v>-14.292502986400001</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1188,7 +1334,7 @@
         <v>-14.291688559400001</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1208,7 +1354,7 @@
         <v>-14.290026367999999</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1228,7 +1374,7 @@
         <v>-14.289292319699999</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1248,7 +1394,7 @@
         <v>-14.289830261500001</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1268,7 +1414,7 @@
         <v>-14.288869749</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1288,7 +1434,7 @@
         <v>-14.2897215509</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1316,22 +1462,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1348,7 +1494,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1359,7 +1505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1370,7 +1516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1381,7 +1527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1398,7 +1544,7 @@
         <v>-14.2907720315</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1415,7 +1561,7 @@
         <v>-14.2913519202</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1432,7 +1578,7 @@
         <v>-14.291131522500001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1449,7 +1595,7 @@
         <v>-14.2897126905</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1466,7 +1612,7 @@
         <v>-14.2909125717</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1483,7 +1629,7 @@
         <v>-14.2897257644</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1500,7 +1646,7 @@
         <v>-14.2926303124</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1517,7 +1663,7 @@
         <v>-14.2925835986</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1534,7 +1680,7 @@
         <v>-14.2920813863</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1551,7 +1697,7 @@
         <v>-14.289224685100001</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1568,7 +1714,7 @@
         <v>-14.2904269686</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1585,7 +1731,7 @@
         <v>-14.289821587900001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1602,7 +1748,7 @@
         <v>-14.291256342300001</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1619,7 +1765,7 @@
         <v>-14.291420175500001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1636,7 +1782,7 @@
         <v>-14.290662125300001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1653,7 +1799,7 @@
         <v>-14.2915457557</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1670,7 +1816,7 @@
         <v>-14.2903972341</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1687,7 +1833,7 @@
         <v>-14.288742795199999</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1704,7 +1850,7 @@
         <v>-14.293183777499999</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1721,7 +1867,7 @@
         <v>-14.292502986400001</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1738,7 +1884,7 @@
         <v>-14.291688559400001</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1755,7 +1901,7 @@
         <v>-14.290026367999999</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1772,7 +1918,7 @@
         <v>-14.289292319699999</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1789,7 +1935,7 @@
         <v>-14.289830261500001</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1806,7 +1952,7 @@
         <v>-14.288869749</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1823,7 +1969,7 @@
         <v>-14.2897215509</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1848,27 +1994,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2:N13"/>
+      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="12" max="14" width="23.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="12" max="14" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1906,7 +2052,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1938,20 +2084,20 @@
       <c r="K2">
         <v>3.0962697664007144</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="7">
         <v>3.6494891514638068</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="7">
         <v>31.970476312297155</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="7">
         <v>64.380034536239037</v>
       </c>
       <c r="O2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1985,20 +2131,20 @@
       <c r="K3">
         <v>9.1393304792808614</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="7">
         <v>4.190185331624555</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="7">
         <v>30.860478644597727</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="7">
         <v>64.949336023777718</v>
       </c>
       <c r="O3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2030,20 +2176,20 @@
       <c r="K4">
         <v>1.2862981286298081</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="7">
         <v>3.882555388255545</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="7">
         <v>81.677357137735768</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="7">
         <v>14.440087474008681</v>
       </c>
       <c r="O4">
         <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2077,20 +2223,20 @@
       <c r="K5">
         <v>11.997980308003035</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="7">
         <v>4.6563998990153657</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="7">
         <v>82.467306235799057</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="7">
         <v>12.876293865185577</v>
       </c>
       <c r="O5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2122,20 +2268,20 @@
       <c r="K6">
         <v>24.446556770142827</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="7">
         <v>5.1060609850664003</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="7">
         <v>77.357843259874457</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="7">
         <v>17.536095755059151</v>
       </c>
       <c r="O6">
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2169,20 +2315,20 @@
       <c r="K7">
         <v>26.074550923453177</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="7">
         <v>4.9630337615607525</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="7">
         <v>82.013345795968817</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="7">
         <v>13.023620442470435</v>
       </c>
       <c r="O7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2214,20 +2360,20 @@
       <c r="K8">
         <v>8.1879002393763898</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="7">
         <v>4.4325551895574691</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="7">
         <v>85.773461955521029</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="7">
         <v>9.7939828549215058</v>
       </c>
       <c r="O8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2261,20 +2407,20 @@
       <c r="K9">
         <v>5.0968563146466401</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="7">
         <v>3.8774615195370856</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="7">
         <v>88.346169068018696</v>
       </c>
-      <c r="N9" s="11">
+      <c r="N9" s="7">
         <v>7.7763694124442289</v>
       </c>
       <c r="O9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2306,20 +2452,20 @@
       <c r="K10">
         <v>9.8527492647202148</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="7">
         <v>4.2899437097056943</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="7">
         <v>86.801269940203667</v>
       </c>
-      <c r="N10" s="11">
+      <c r="N10" s="7">
         <v>8.9087863500906348</v>
       </c>
       <c r="O10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2351,20 +2497,20 @@
       <c r="K11">
         <v>2.2622748177637266</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="7">
         <v>3.8583192452418764</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="7">
         <v>83.537865154241857</v>
       </c>
-      <c r="N11" s="11">
+      <c r="N11" s="7">
         <v>12.603815600516258</v>
       </c>
       <c r="O11">
         <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2396,20 +2542,20 @@
       <c r="K12">
         <v>4.07519792830103</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="7">
         <v>4.0010674784774407</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="7">
         <v>79.726982495329864</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="7">
         <v>16.271950026192691</v>
       </c>
       <c r="O12">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2443,13 +2589,13 @@
       <c r="K13">
         <v>2.0573410963481171</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="7">
         <v>3.9270049123106379</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="7">
         <v>80.640214122715321</v>
       </c>
-      <c r="N13" s="11">
+      <c r="N13" s="7">
         <v>15.432780964974029</v>
       </c>
       <c r="O13">
@@ -2463,75 +2609,95 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1:S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="15" max="15" width="9.109375" style="28"/>
+    <col min="16" max="19" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:19" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="P1" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="R1" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="S1" s="27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="9">
         <v>8.7143999999999977</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="10">
         <v>4.0530615991921142</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="10">
         <v>85.653791425686236</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="10">
         <v>10.293146975121649</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="9" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="11">
@@ -2542,191 +2708,290 @@
         <f>B3/(B2+B3)*100</f>
         <v>11.997980308003035</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="12">
         <f>(C2*$G2/100)+(C3*$H2/100)</f>
         <v>4.6563998990153657</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="12">
         <f>(D2*$G2/100)+(D3*$H2/100)</f>
         <v>82.467306235799057</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="12">
         <f>(E2*$G2/100)+(E3*$H2/100)</f>
         <v>12.876293865185577</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="12">
         <f>(K2+J2+I2)</f>
         <v>100</v>
       </c>
-      <c r="N2">
+      <c r="M2" s="9"/>
+      <c r="N2" s="13">
         <f>H2*E3/100</f>
         <v>3.8181166372128326</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="O2" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="P2" s="7">
+        <f>MAX($I2,$I4,$I6)</f>
+        <v>5.1060609850664003</v>
+      </c>
+      <c r="Q2" s="7">
+        <f>MIN($I2,$I4,$I6)</f>
+        <v>4.6563998990153657</v>
+      </c>
+      <c r="R2" s="7">
+        <f>MEDIAN($I2,$I4,$I6)</f>
+        <v>4.9630337615607525</v>
+      </c>
+      <c r="S2" s="7">
+        <f>AVERAGE($I2,$I4,$I6)</f>
+        <v>4.9084982152141725</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="15">
         <v>1.1881000000000004</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="16">
         <v>9.0817271273460953</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="16">
         <v>59.095278175237816</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="16">
         <v>31.822994697416089</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" s="7">
+        <f>MAX($J2,$J4,$J6)</f>
+        <v>82.467306235799057</v>
+      </c>
+      <c r="Q3" s="7">
+        <f>MIN($J2,$J4,$J6)</f>
+        <v>77.357843259874457</v>
+      </c>
+      <c r="R3" s="7">
+        <f>MEDIAN($J2,$J4,$J6)</f>
+        <v>82.013345795968817</v>
+      </c>
+      <c r="S3" s="7">
+        <f>AVERAGE($J2,$J4,$J6)</f>
+        <v>80.612831763880777</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="15">
         <v>12.081599999999998</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="16">
         <v>4.1277645344987377</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="16">
         <v>85.808916037610928</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="16">
         <v>10.063319427890335</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="17">
         <f>B4/(B4+B5)*100</f>
         <v>75.55344322985718</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="17">
         <f>B5/(B4+B5)*100</f>
         <v>24.446556770142827</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="19">
         <f>(C4*$G4/100)+(C5*$H4/100)</f>
         <v>5.1060609850664003</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="19">
         <f>(D4*$G4/100)+(D5*$H4/100)</f>
         <v>77.357843259874457</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="19">
         <f>(E4*$G4/100)+(E5*$H4/100)</f>
         <v>17.536095755059151</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="19">
         <f>(K4+J4+I4)</f>
         <v>100.00000000000001</v>
       </c>
-      <c r="N4">
+      <c r="M4" s="15"/>
+      <c r="N4" s="18">
         <f>H4*E5/100</f>
         <v>9.9329114240688359</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="O4" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="P4" s="7">
+        <f>MAX($K2,$K4,$K6)</f>
+        <v>17.536095755059151</v>
+      </c>
+      <c r="Q4" s="7">
+        <f>MIN($K2,$K4,$K6)</f>
+        <v>12.876293865185577</v>
+      </c>
+      <c r="R4" s="7">
+        <f>MEDIAN($K2,$K4,$K6)</f>
+        <v>13.023620442470435</v>
+      </c>
+      <c r="S4" s="7">
+        <f>AVERAGE($K2,$K4,$K6)</f>
+        <v>14.478670020905055</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="15">
         <v>3.9091999999999985</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="16">
         <v>8.1295405709607707</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="16">
         <v>51.239332855827328</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="16">
         <v>40.631126573211901</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F5" s="15"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="18"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="15">
         <v>10.519000000000002</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="16">
         <v>4.2703679056944681</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="16">
         <v>86.904810343188515</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="16">
         <v>8.8248217511170175</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="17">
         <f>B6/(B6+B7)*100</f>
         <v>73.925449076546826</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="17">
         <f>B7/(B6+B7)*100</f>
         <v>26.074550923453177</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="19">
         <f>(C6*$G6/100)+(C7*$H6/100)</f>
         <v>4.9630337615607525</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="19">
         <f>(D6*$G6/100)+(D7*$H6/100)</f>
         <v>82.013345795968817</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="19">
         <f>(E6*$G6/100)+(E7*$H6/100)</f>
         <v>13.023620442470435</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="19">
         <f>(K6+J6+I6)</f>
         <v>100</v>
       </c>
-      <c r="N6">
+      <c r="M6" s="15"/>
+      <c r="N6" s="18">
         <f>H6*E7/100</f>
         <v>6.4998313327523958</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="21">
         <v>3.7102000000000004</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="22">
         <v>6.9268503045658303</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="22">
         <v>68.145275187321289</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="22">
         <v>24.927874508112879</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F7" s="21"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="24"/>
+      <c r="P7" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q7" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="R7" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="S7" s="27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="9">
         <v>12.121300000000002</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="10">
         <v>3.4138252497669543</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="10">
         <v>32.591231963568283</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="10">
         <v>63.994942786664772</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="11">
@@ -2737,191 +3002,290 @@
         <f>B9/(B8+B9)*100</f>
         <v>3.0962697664007144</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="12">
         <f>(C8*$G8/100)+(C9*$H8/100)</f>
         <v>3.6494891514638068</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="12">
         <f>(D8*$G8/100)+(D9*$H8/100)</f>
         <v>31.970476312297155</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="12">
         <f>(E8*$G8/100)+(E9*$H8/100)</f>
         <v>64.380034536239037</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="12">
         <f>(K8+J8+I8)</f>
         <v>100</v>
       </c>
-      <c r="N8">
+      <c r="M8" s="9"/>
+      <c r="N8" s="13">
         <f>H8*E9/100</f>
         <v>2.3665478151032091</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="O8" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="P8" s="7">
+        <f>MAX($I8,$I10,$I12)</f>
+        <v>4.190185331624555</v>
+      </c>
+      <c r="Q8" s="7">
+        <f>MIN($I8,$I10,$I12)</f>
+        <v>3.6494891514638068</v>
+      </c>
+      <c r="R8" s="7">
+        <f>MEDIAN($I8,$I10,$I12)</f>
+        <v>3.882555388255545</v>
+      </c>
+      <c r="S8" s="7">
+        <f>AVERAGE($I8,$I10,$I12)</f>
+        <v>3.9074099571146355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="15">
         <v>0.38729999999999976</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="16">
         <v>11.025045184611409</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="16">
         <v>12.542731732507031</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="16">
         <v>76.432223082881549</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="F9" s="15"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="P9" s="7">
+        <f>MAX($J8,$J10,$J12)</f>
+        <v>81.677357137735768</v>
+      </c>
+      <c r="Q9" s="7">
+        <f>MIN($J8,$J10,$J12)</f>
+        <v>30.860478644597727</v>
+      </c>
+      <c r="R9" s="7">
+        <f>MEDIAN($J8,$J10,$J12)</f>
+        <v>31.970476312297155</v>
+      </c>
+      <c r="S9" s="7">
+        <f>AVERAGE($J8,$J10,$J12)</f>
+        <v>48.169437364876877</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="15">
         <v>9.9964000000000013</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="16">
         <v>3.5622824216718154</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="16">
         <v>33.172101956704381</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="16">
         <v>63.265615621623802</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="17">
         <f>B10/(B10+B11)*100</f>
         <v>90.860669520719142</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="17">
         <f>B11/(B10+B11)*100</f>
         <v>9.1393304792808614</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="19">
         <f>(C10*$G10/100)+(C11*$H10/100)</f>
         <v>4.190185331624555</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="19">
         <f>(D10*$G10/100)+(D11*$H10/100)</f>
         <v>30.860478644597727</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="19">
         <f>(E10*$G10/100)+(E11*$H10/100)</f>
         <v>64.949336023777718</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="19">
         <f>(K10+J10+I10)</f>
         <v>100</v>
       </c>
-      <c r="N10">
+      <c r="M10" s="15"/>
+      <c r="N10" s="18">
         <f>H10*E11/100</f>
         <v>7.4657740935656536</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="O10" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="P10" s="7">
+        <f>MAX($K8,$K10,$K12)</f>
+        <v>64.949336023777718</v>
+      </c>
+      <c r="Q10" s="7">
+        <f>MIN($K8,$K10,$K12)</f>
+        <v>14.440087474008681</v>
+      </c>
+      <c r="R10" s="7">
+        <f>MEDIAN($K8,$K10,$K12)</f>
+        <v>64.380034536239037</v>
+      </c>
+      <c r="S10" s="7">
+        <f>AVERAGE($K8,$K10,$K12)</f>
+        <v>47.923152678008478</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="15">
         <v>1.0055000000000014</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="16">
         <v>10.432620586772801</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="16">
         <v>7.8789656887121566</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="16">
         <v>81.688413724515044</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="18"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="15">
         <v>13.767600000000002</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="16">
         <v>3.7624567825910149</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="16">
         <v>82.339354716871554</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="16">
         <v>13.898188500537431</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="17">
         <f>B12/(B12+B13)*100</f>
         <v>98.713701871370191</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="17">
         <f>B13/(B12+B13)*100</f>
         <v>1.2862981286298081</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="19">
         <f>(C12*$G12/100)+(C13*$H12/100)</f>
         <v>3.882555388255545</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="19">
         <f>(D12*$G12/100)+(D13*$H12/100)</f>
         <v>81.677357137735768</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="19">
         <f>(E12*$G12/100)+(E13*$H12/100)</f>
         <v>14.440087474008681</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="19">
         <f>(K12+J12+I12)</f>
         <v>99.999999999999986</v>
       </c>
-      <c r="N12">
+      <c r="M12" s="15"/>
+      <c r="N12" s="18">
         <f>H12*E13/100</f>
         <v>0.72067111206710466</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="21">
         <v>0.17939999999999934</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="22">
         <v>13.099219620958966</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="22">
         <v>30.874024526198522</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="22">
         <v>56.026755852842513</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="F13" s="21"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="24"/>
+      <c r="P13" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q13" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="R13" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="S13" s="27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="9">
         <v>10.753300000000001</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="10">
         <v>3.7225781853012694</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="10">
         <v>84.415974631043468</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="10">
         <v>11.861447183655262</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G14" s="11">
@@ -2932,191 +3296,290 @@
         <f>B15/(B14+B15)*100</f>
         <v>2.2622748177637266</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="12">
         <f>(C14*$G14/100)+(C15*$H14/100)</f>
         <v>3.8583192452418764</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="12">
         <f>(D14*$G14/100)+(D15*$H14/100)</f>
         <v>83.537865154241857</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="12">
         <f>(E14*$G14/100)+(E15*$H14/100)</f>
         <v>12.603815600516258</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="12">
         <f>(K14+J14+I14)</f>
         <v>99.999999999999986</v>
       </c>
-      <c r="N14">
+      <c r="M14" s="9"/>
+      <c r="N14" s="13">
         <f>H14*E15/100</f>
         <v>1.0107069495191754</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="O14" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="P14" s="7">
+        <f>MAX($I14,$I16,$I18)</f>
+        <v>4.0010674784774407</v>
+      </c>
+      <c r="Q14" s="7">
+        <f>MIN($I14,$I16,$I18)</f>
+        <v>3.8583192452418764</v>
+      </c>
+      <c r="R14" s="7">
+        <f>MEDIAN($I14,$I16,$I18)</f>
+        <v>3.9270049123106379</v>
+      </c>
+      <c r="S14" s="7">
+        <f>AVERAGE($I14,$I16,$I18)</f>
+        <v>3.9287972120099846</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="15">
         <v>0.24890000000000079</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="16">
         <v>9.7227802330254587</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="16">
         <v>45.600642828445658</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="16">
         <v>44.676576938528882</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="F15" s="15"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="P15" s="7">
+        <f>MAX($J14,$J16,$J18)</f>
+        <v>83.537865154241857</v>
+      </c>
+      <c r="Q15" s="7">
+        <f>MIN($J14,$J16,$J18)</f>
+        <v>79.726982495329864</v>
+      </c>
+      <c r="R15" s="7">
+        <f>MEDIAN($J14,$J16,$J18)</f>
+        <v>80.640214122715321</v>
+      </c>
+      <c r="S15" s="7">
+        <f>AVERAGE($J14,$J16,$J18)</f>
+        <v>81.301687257429009</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="15">
         <v>9.7049999999999983</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="16">
         <v>3.6836682122617024</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="16">
         <v>81.51884595569301</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="16">
         <v>14.797485832045288</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="17">
         <f>B16/(B16+B17)*100</f>
         <v>95.924802071698963</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="17">
         <f>B17/(B16+B17)*100</f>
         <v>4.07519792830103</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="19">
         <f>(C16*$G16/100)+(C17*$H16/100)</f>
         <v>4.0010674784774407</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="19">
         <f>(D16*$G16/100)+(D17*$H16/100)</f>
         <v>79.726982495329864</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="19">
         <f>(E16*$G16/100)+(E17*$H16/100)</f>
         <v>16.271950026192691</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="19">
         <f>(K16+J16+I16)</f>
         <v>100</v>
       </c>
-      <c r="N16">
+      <c r="M16" s="15"/>
+      <c r="N16" s="18">
         <f>H16*E17/100</f>
         <v>2.0774910302155525</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="O16" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="P16" s="7">
+        <f>MAX($K14,$K16,$K18)</f>
+        <v>16.271950026192691</v>
+      </c>
+      <c r="Q16" s="7">
+        <f>MIN($K14,$K16,$K18)</f>
+        <v>12.603815600516258</v>
+      </c>
+      <c r="R16" s="7">
+        <f>MEDIAN($K14,$K16,$K18)</f>
+        <v>15.432780964974029</v>
+      </c>
+      <c r="S16" s="7">
+        <f>AVERAGE($K14,$K16,$K18)</f>
+        <v>14.769515530560993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="15">
         <v>0.41230000000000011</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="16">
         <v>11.472228959495485</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="16">
         <v>37.548872180451632</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="16">
         <v>50.97889886005288</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="F17" s="15"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="18"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="15">
         <v>13.777299999999999</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="16">
         <v>3.7634369578945046</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="16">
         <v>81.515231576578856</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="16">
         <v>14.721331465526639</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="17">
         <f>B18/(B18+B19)*100</f>
         <v>97.942658903651875</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="17">
         <f>B19/(B18+B19)*100</f>
         <v>2.0573410963481171</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="19">
         <f>(C18*$G18/100)+(C19*$H18/100)</f>
         <v>3.9270049123106379</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="19">
         <f>(D18*$G18/100)+(D19*$H18/100)</f>
         <v>80.640214122715321</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="19">
         <f>(E18*$G18/100)+(E19*$H18/100)</f>
         <v>15.432780964974029</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="19">
         <f>(K18+J18+I18)</f>
         <v>99.999999999999986</v>
       </c>
-      <c r="N18">
+      <c r="M18" s="15"/>
+      <c r="N18" s="18">
         <f>H18*E19/100</f>
         <v>1.0143175016172981</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="21">
         <v>0.28940000000000055</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="22">
         <v>11.713890808569753</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="22">
         <v>38.983759502418437</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="22">
         <v>49.302349689011812</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="F19" s="21"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="24"/>
+      <c r="P19" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q19" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="R19" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="S19" s="27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="9">
         <v>8.9750000000000014</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="10">
         <v>4.1526462395543371</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="10">
         <v>87.087064066852378</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="10">
         <v>8.7602896935932861</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="9" t="s">
         <v>16</v>
       </c>
       <c r="G20" s="11">
@@ -3127,188 +3590,274 @@
         <f>B21/(B20+B21)*100</f>
         <v>8.1879002393763898</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="12">
         <f>(C20*$G20/100)+(C21*$H20/100)</f>
         <v>4.4325551895574691</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="12">
         <f>(D20*$G20/100)+(D21*$H20/100)</f>
         <v>85.773461955521029</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="12">
         <f>(E20*$G20/100)+(E21*$H20/100)</f>
         <v>9.7939828549215058</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="12">
         <f>(K20+J20+I20)</f>
         <v>100</v>
       </c>
-      <c r="N20">
+      <c r="M20" s="9"/>
+      <c r="N20" s="13">
         <f>H20*E21/100</f>
         <v>1.7509769421200077</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="O20" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="P20" s="7">
+        <f>MAX($I20,$I22,$I24)</f>
+        <v>4.4325551895574691</v>
+      </c>
+      <c r="Q20" s="7">
+        <f>MIN($I20,$I22,$I24)</f>
+        <v>3.8774615195370856</v>
+      </c>
+      <c r="R20" s="7">
+        <f>MEDIAN($I20,$I22,$I24)</f>
+        <v>4.2899437097056943</v>
+      </c>
+      <c r="S20" s="7">
+        <f>AVERAGE($I20,$I22,$I24)</f>
+        <v>4.1999868062667494</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="15">
         <v>0.80039999999999978</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="16">
         <v>7.5712143928034878</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="16">
         <v>71.043853073463467</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="16">
         <v>21.384932533733046</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="F21" s="15"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="P21" s="7">
+        <f>MAX($J20,$J22,$J24)</f>
+        <v>88.346169068018696</v>
+      </c>
+      <c r="Q21" s="7">
+        <f>MIN($J20,$J22,$J24)</f>
+        <v>85.773461955521029</v>
+      </c>
+      <c r="R21" s="7">
+        <f>MEDIAN($J20,$J22,$J24)</f>
+        <v>86.801269940203667</v>
+      </c>
+      <c r="S21" s="7">
+        <f>AVERAGE($J20,$J22,$J24)</f>
+        <v>86.973633654581135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="15">
         <v>8.872399999999999</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="16">
         <v>3.6686804021460002</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="16">
         <v>89.045895135476314</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="16">
         <v>7.2854244623776854</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="17">
         <f>B22/(B22+B23)*100</f>
         <v>94.903143685353371</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H22" s="17">
         <f>B23/(B22+B23)*100</f>
         <v>5.0968563146466401</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="19">
         <f>(C22*$G22/100)+(C23*$H22/100)</f>
         <v>3.8774615195370856</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="19">
         <f>(D22*$G22/100)+(D23*$H22/100)</f>
         <v>88.346169068018696</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="19">
         <f>(E22*$G22/100)+(E23*$H22/100)</f>
         <v>7.7763694124442289</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L22" s="19">
         <f>(K22+J22+I22)</f>
         <v>100</v>
       </c>
-      <c r="N22">
+      <c r="M22" s="15"/>
+      <c r="N22" s="18">
         <f>H22*E23/100</f>
         <v>0.86227256682605047</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="O22" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="P22" s="7">
+        <f>MAX($K20,$K22,$K24)</f>
+        <v>9.7939828549215058</v>
+      </c>
+      <c r="Q22" s="7">
+        <f>MIN($K20,$K22,$K24)</f>
+        <v>7.7763694124442289</v>
+      </c>
+      <c r="R22" s="7">
+        <f>MEDIAN($K20,$K22,$K24)</f>
+        <v>8.9087863500906348</v>
+      </c>
+      <c r="S22" s="7">
+        <f>AVERAGE($K20,$K22,$K24)</f>
+        <v>8.8263795391521231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="15">
         <v>0.4764999999999997</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="16">
         <v>7.7649527806927239</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="16">
         <v>75.317313746064741</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="16">
         <v>16.917733473242535</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="F23" s="15"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="18"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="15">
         <v>9.2564999999999991</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="16">
         <v>4.0576891913790165</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="16">
         <v>87.678182898503721</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="16">
         <v>8.2641279101172636</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="17">
         <f>B24/(B24+B25)*100</f>
         <v>90.147250735279783</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="17">
         <f>B25/(B24+B25)*100</f>
         <v>9.8527492647202148</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="19">
         <f>(C24*$G24/100)+(C25*$H24/100)</f>
         <v>4.2899437097056943</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="19">
         <f>(D24*$G24/100)+(D25*$H24/100)</f>
         <v>86.801269940203667</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="19">
         <f>(E24*$G24/100)+(E25*$H24/100)</f>
         <v>8.9087863500906348</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24" s="19">
         <f>(K24+J24+I24)</f>
         <v>100</v>
       </c>
-      <c r="N24">
+      <c r="M24" s="15"/>
+      <c r="N24" s="18">
         <f>H24*E25/100</f>
         <v>1.4589022418729889</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="21">
         <v>1.0117000000000012</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="22">
         <v>6.414945141840608</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="22">
         <v>78.777997430067856</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="22">
         <v>14.807057428091536</v>
       </c>
-      <c r="N25" t="s">
+      <c r="F25" s="21"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="24" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>80</v>
       </c>
-      <c r="N26" s="9">
+      <c r="N26" s="5">
         <f>MAX(N2,N4,N6,N8,N10,N12,N14,N16,N18,N20,N22,N24)</f>
         <v>9.9329114240688359</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E27" s="9">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="E27" s="5">
         <f>MAX(E3,E5,E7,E9,E11,E13,E15,E17,E19,E21,E23,E25)</f>
         <v>81.688413724515044</v>
       </c>
@@ -3316,17 +3865,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>81</v>
       </c>
-      <c r="N28" s="9">
+      <c r="N28" s="5">
         <f>MIN(N4,N6,N8,N10,N12,N14,N16,N18,N20,N22,N24,N2)</f>
         <v>0.72067111206710466</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E29" s="9">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="E29" s="5">
         <f>MIN(E5,E7,E9,E11,E13,E15,E17,E19,E21,E23,E25,E3)</f>
         <v>14.807057428091536</v>
       </c>
@@ -3334,17 +3883,17 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
         <v>82</v>
       </c>
-      <c r="N30" s="9">
+      <c r="N30" s="5">
         <f>MEDIAN(N6,N8,N10,N12,N14,N16,N18,N20,N22,N24,N2,N4)</f>
         <v>1.9142339861677802</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E31" s="9">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="E31" s="5">
         <f>MEDIAN(E7,E9,E11,E13,E15,E17,E19,E21,E23,E25,E3,E5)</f>
         <v>42.653851755870392</v>
       </c>
@@ -3352,22 +3901,23 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E32" t="s">
         <v>83</v>
       </c>
-      <c r="N32" s="9">
+      <c r="N32" s="5">
         <f>AVERAGE(N8,N10,N12,N14,N16,N18,N20,N22,N24,N2,N4,N6)</f>
         <v>3.2482099705784253</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="9">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="5">
         <f>AVERAGE(E9,E11,E13,E15,E17,E19,E21,E23,E25,E3,E5,E7)</f>
         <v>42.466411446803384</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>